<commit_message>
FPGA V25. Adds 2 HPF controls for future TX signal path. No negative impact for normal operation.
</commit_message>
<xml_diff>
--- a/FPGA/documentation/FPGA Pins.xlsx
+++ b/FPGA/documentation/FPGA Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xilinxdesigns\Saturn\FPGA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBD8A1E-6C65-4DB6-A97C-5A8D4028341E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C9C35D-1D77-413D-BCCC-EF0C406E3503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31275" yWindow="810" windowWidth="6465" windowHeight="16965" xr2:uid="{CA1EC664-29DC-4727-9958-A9C744273A35}"/>
+    <workbookView xWindow="15240" yWindow="720" windowWidth="23055" windowHeight="16965" xr2:uid="{CA1EC664-29DC-4727-9958-A9C744273A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="608">
   <si>
     <t>Banks 12, 33 prohibited as potential enabler for Saturn to target XC7A100T device</t>
   </si>
@@ -1842,6 +1842,24 @@
   </si>
   <si>
     <t>CODEC_RESETN[0]</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>HPF_SEL1</t>
+  </si>
+  <si>
+    <t>HPF_SEL2</t>
+  </si>
+  <si>
+    <t>controls TX HPF; selected if 1. 50MHz only</t>
+  </si>
+  <si>
+    <t>controls TX HPF; selected if 0. 50MHz only</t>
   </si>
 </sst>
 </file>
@@ -2236,15 +2254,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9BB1FE-8FBD-4D1A-B469-03ACC29AE053}">
-  <dimension ref="A2:F218"/>
+  <dimension ref="A2:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="6" max="6" width="37.140625" customWidth="1"/>
@@ -3458,7 +3476,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>259</v>
       </c>
@@ -3478,60 +3496,56 @@
         <v>262</v>
       </c>
     </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>602</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" t="s">
+        <v>604</v>
+      </c>
+      <c r="D79" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" t="s">
+        <v>16</v>
+      </c>
+      <c r="F79" t="s">
+        <v>606</v>
+      </c>
+    </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>140</v>
-      </c>
-      <c r="B81" t="s">
-        <v>487</v>
-      </c>
-      <c r="C81" t="s">
-        <v>141</v>
-      </c>
-      <c r="D81" t="s">
-        <v>135</v>
-      </c>
-      <c r="E81" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" t="s">
-        <v>214</v>
+        <v>603</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" t="s">
+        <v>605</v>
+      </c>
+      <c r="D80" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" t="s">
+        <v>16</v>
+      </c>
+      <c r="F80" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>142</v>
-      </c>
-      <c r="B82" t="s">
-        <v>504</v>
-      </c>
-      <c r="C82" t="s">
-        <v>143</v>
-      </c>
-      <c r="D82" t="s">
-        <v>135</v>
-      </c>
-      <c r="E82" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B83" t="s">
-        <v>564</v>
+        <v>487</v>
       </c>
       <c r="C83" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D83" t="s">
         <v>135</v>
@@ -3540,18 +3554,18 @@
         <v>16</v>
       </c>
       <c r="F83" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B84" t="s">
         <v>504</v>
       </c>
       <c r="C84" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D84" t="s">
         <v>135</v>
@@ -3560,18 +3574,18 @@
         <v>16</v>
       </c>
       <c r="F84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B85" t="s">
-        <v>506</v>
+        <v>564</v>
       </c>
       <c r="C85" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D85" t="s">
         <v>135</v>
@@ -3579,16 +3593,19 @@
       <c r="E85" t="s">
         <v>16</v>
       </c>
+      <c r="F85" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B86" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C86" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D86" t="s">
         <v>135</v>
@@ -3596,16 +3613,19 @@
       <c r="E86" t="s">
         <v>16</v>
       </c>
+      <c r="F86" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B87" t="s">
-        <v>130</v>
+        <v>506</v>
       </c>
       <c r="C87" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D87" t="s">
         <v>135</v>
@@ -3616,13 +3636,13 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B88" t="s">
-        <v>267</v>
+        <v>510</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D88" t="s">
         <v>135</v>
@@ -3633,13 +3653,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B89" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D89" t="s">
         <v>135</v>
@@ -3650,13 +3670,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C90" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D90" t="s">
         <v>135</v>
@@ -3667,13 +3687,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="C91" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D91" t="s">
         <v>135</v>
@@ -3684,13 +3704,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B92" t="s">
-        <v>509</v>
+        <v>265</v>
       </c>
       <c r="C92" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D92" t="s">
         <v>135</v>
@@ -3701,13 +3721,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B93" t="s">
-        <v>505</v>
+        <v>128</v>
       </c>
       <c r="C93" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D93" t="s">
         <v>135</v>
@@ -3718,13 +3738,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B94" t="s">
-        <v>160</v>
+        <v>509</v>
       </c>
       <c r="C94" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D94" t="s">
         <v>135</v>
@@ -3735,13 +3755,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B95" t="s">
-        <v>210</v>
+        <v>505</v>
       </c>
       <c r="C95" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D95" t="s">
         <v>135</v>
@@ -3752,13 +3772,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B96" t="s">
-        <v>396</v>
+        <v>160</v>
       </c>
       <c r="C96" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D96" t="s">
         <v>135</v>
@@ -3769,13 +3789,13 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B97" t="s">
-        <v>398</v>
+        <v>210</v>
       </c>
       <c r="C97" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D97" t="s">
         <v>135</v>
@@ -3786,13 +3806,13 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B98" t="s">
-        <v>508</v>
+        <v>396</v>
       </c>
       <c r="C98" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D98" t="s">
         <v>135</v>
@@ -3803,13 +3823,13 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
-        <v>507</v>
+        <v>398</v>
       </c>
       <c r="C99" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D99" t="s">
         <v>135</v>
@@ -3820,13 +3840,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B100" t="s">
-        <v>224</v>
+        <v>508</v>
       </c>
       <c r="C100" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D100" t="s">
         <v>135</v>
@@ -3837,13 +3857,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>180</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>504</v>
+        <v>176</v>
+      </c>
+      <c r="B101" t="s">
+        <v>507</v>
       </c>
       <c r="C101" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D101" t="s">
         <v>135</v>
@@ -3851,19 +3871,16 @@
       <c r="E101" t="s">
         <v>16</v>
       </c>
-      <c r="F101" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>182</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>504</v>
+        <v>178</v>
+      </c>
+      <c r="B102" t="s">
+        <v>224</v>
       </c>
       <c r="C102" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D102" t="s">
         <v>135</v>
@@ -3874,13 +3891,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C103" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D103" t="s">
         <v>135</v>
@@ -3888,16 +3905,19 @@
       <c r="E103" t="s">
         <v>16</v>
       </c>
+      <c r="F103" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C104" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D104" t="s">
         <v>135</v>
@@ -3908,13 +3928,13 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C105" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D105" t="s">
         <v>135</v>
@@ -3925,13 +3945,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C106" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D106" t="s">
         <v>135</v>
@@ -3942,13 +3962,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C107" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D107" t="s">
         <v>135</v>
@@ -3959,13 +3979,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C108" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D108" t="s">
         <v>135</v>
@@ -3976,13 +3996,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C109" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D109" t="s">
         <v>135</v>
@@ -3993,13 +4013,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C110" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D110" t="s">
         <v>135</v>
@@ -4010,13 +4030,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D111" t="s">
         <v>135</v>
@@ -4027,13 +4047,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C112" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D112" t="s">
         <v>135</v>
@@ -4044,13 +4064,13 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C113" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D113" t="s">
         <v>135</v>
@@ -4061,13 +4081,13 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C114" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D114" t="s">
         <v>135</v>
@@ -4078,13 +4098,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C115" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D115" t="s">
         <v>135</v>
@@ -4095,13 +4115,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>504</v>
       </c>
       <c r="C116" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D116" t="s">
         <v>135</v>
@@ -4110,60 +4130,54 @@
         <v>16</v>
       </c>
     </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>208</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C117" t="s">
+        <v>209</v>
+      </c>
+      <c r="D117" t="s">
+        <v>135</v>
+      </c>
+      <c r="E117" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>218</v>
-      </c>
-      <c r="B119" t="s">
-        <v>563</v>
-      </c>
-      <c r="C119" t="s">
-        <v>219</v>
-      </c>
-      <c r="D119" t="s">
-        <v>21</v>
-      </c>
-      <c r="E119" t="s">
-        <v>16</v>
-      </c>
-      <c r="F119" t="s">
-        <v>230</v>
+        <v>210</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="C118" t="s">
+        <v>211</v>
+      </c>
+      <c r="D118" t="s">
+        <v>135</v>
+      </c>
+      <c r="E118" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>220</v>
-      </c>
-      <c r="B120" t="s">
-        <v>566</v>
-      </c>
-      <c r="C120" t="s">
-        <v>221</v>
-      </c>
-      <c r="D120" t="s">
-        <v>21</v>
-      </c>
-      <c r="E120" t="s">
-        <v>16</v>
-      </c>
-      <c r="F120" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B121" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C121" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D121" t="s">
         <v>21</v>
@@ -4172,15 +4186,18 @@
         <v>16</v>
       </c>
       <c r="F121" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>224</v>
+        <v>220</v>
+      </c>
+      <c r="B122" t="s">
+        <v>566</v>
       </c>
       <c r="C122" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D122" t="s">
         <v>21</v>
@@ -4189,15 +4206,18 @@
         <v>16</v>
       </c>
       <c r="F122" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>226</v>
+        <v>222</v>
+      </c>
+      <c r="B123" t="s">
+        <v>565</v>
       </c>
       <c r="C123" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D123" t="s">
         <v>21</v>
@@ -4206,15 +4226,15 @@
         <v>16</v>
       </c>
       <c r="F123" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C124" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D124" t="s">
         <v>21</v>
@@ -4223,63 +4243,57 @@
         <v>16</v>
       </c>
       <c r="F124" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>226</v>
+      </c>
+      <c r="C125" t="s">
+        <v>227</v>
+      </c>
+      <c r="D125" t="s">
+        <v>21</v>
+      </c>
+      <c r="E125" t="s">
+        <v>16</v>
+      </c>
+      <c r="F125" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>265</v>
-      </c>
-      <c r="B127" t="s">
-        <v>582</v>
-      </c>
-      <c r="C127" t="s">
-        <v>266</v>
-      </c>
-      <c r="D127" t="s">
-        <v>21</v>
-      </c>
-      <c r="E127" t="s">
-        <v>16</v>
-      </c>
-      <c r="F127" t="s">
-        <v>277</v>
+        <v>228</v>
+      </c>
+      <c r="C126" t="s">
+        <v>229</v>
+      </c>
+      <c r="D126" t="s">
+        <v>21</v>
+      </c>
+      <c r="E126" t="s">
+        <v>16</v>
+      </c>
+      <c r="F126" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>267</v>
-      </c>
-      <c r="B128" t="s">
-        <v>222</v>
-      </c>
-      <c r="C128" t="s">
-        <v>268</v>
-      </c>
-      <c r="D128" t="s">
-        <v>21</v>
-      </c>
-      <c r="E128" t="s">
-        <v>16</v>
-      </c>
-      <c r="F128" t="s">
-        <v>279</v>
+        <v>249</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B129" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="C129" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D129" t="s">
         <v>21</v>
@@ -4288,18 +4302,18 @@
         <v>16</v>
       </c>
       <c r="F129" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B130" t="s">
-        <v>592</v>
+        <v>222</v>
       </c>
       <c r="C130" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D130" t="s">
         <v>21</v>
@@ -4308,18 +4322,18 @@
         <v>16</v>
       </c>
       <c r="F130" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B131" t="s">
-        <v>322</v>
+        <v>589</v>
       </c>
       <c r="C131" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D131" t="s">
         <v>21</v>
@@ -4328,18 +4342,18 @@
         <v>16</v>
       </c>
       <c r="F131" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B132" t="s">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="C132" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D132" t="s">
         <v>21</v>
@@ -4348,18 +4362,18 @@
         <v>16</v>
       </c>
       <c r="F132" t="s">
-        <v>482</v>
+        <v>281</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
       <c r="B133" t="s">
-        <v>525</v>
+        <v>322</v>
       </c>
       <c r="C133" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
       <c r="D133" t="s">
         <v>21</v>
@@ -4368,18 +4382,18 @@
         <v>16</v>
       </c>
       <c r="F133" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>450</v>
+        <v>275</v>
       </c>
       <c r="B134" t="s">
-        <v>374</v>
+        <v>586</v>
       </c>
       <c r="C134" t="s">
-        <v>451</v>
+        <v>276</v>
       </c>
       <c r="D134" t="s">
         <v>21</v>
@@ -4388,63 +4402,63 @@
         <v>16</v>
       </c>
       <c r="F134" t="s">
-        <v>452</v>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>311</v>
+      </c>
+      <c r="B135" t="s">
+        <v>525</v>
+      </c>
+      <c r="C135" t="s">
+        <v>312</v>
+      </c>
+      <c r="D135" t="s">
+        <v>21</v>
+      </c>
+      <c r="E135" t="s">
+        <v>16</v>
+      </c>
+      <c r="F135" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>289</v>
-      </c>
-      <c r="B137" t="s">
-        <v>575</v>
-      </c>
-      <c r="C137" t="s">
-        <v>290</v>
-      </c>
-      <c r="D137" t="s">
-        <v>21</v>
-      </c>
-      <c r="E137" t="s">
-        <v>16</v>
-      </c>
-      <c r="F137" t="s">
-        <v>595</v>
+        <v>450</v>
+      </c>
+      <c r="B136" t="s">
+        <v>374</v>
+      </c>
+      <c r="C136" t="s">
+        <v>451</v>
+      </c>
+      <c r="D136" t="s">
+        <v>21</v>
+      </c>
+      <c r="E136" t="s">
+        <v>16</v>
+      </c>
+      <c r="F136" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>291</v>
-      </c>
-      <c r="B138" t="s">
-        <v>574</v>
-      </c>
-      <c r="C138" t="s">
-        <v>292</v>
-      </c>
-      <c r="D138" t="s">
-        <v>21</v>
-      </c>
-      <c r="E138" t="s">
-        <v>16</v>
-      </c>
-      <c r="F138" t="s">
-        <v>594</v>
+        <v>288</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B139" t="s">
-        <v>560</v>
+        <v>575</v>
       </c>
       <c r="C139" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D139" t="s">
         <v>21</v>
@@ -4453,18 +4467,18 @@
         <v>16</v>
       </c>
       <c r="F139" t="s">
-        <v>305</v>
+        <v>595</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B140" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C140" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D140" t="s">
         <v>21</v>
@@ -4473,18 +4487,18 @@
         <v>16</v>
       </c>
       <c r="F140" t="s">
-        <v>306</v>
+        <v>594</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B141" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="C141" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D141" t="s">
         <v>21</v>
@@ -4493,157 +4507,157 @@
         <v>16</v>
       </c>
       <c r="F141" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B142" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="C142" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D142" t="s">
         <v>21</v>
       </c>
       <c r="E142" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="F142" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B143" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="C143" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D143" t="s">
         <v>21</v>
       </c>
       <c r="E143" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="F143" t="s">
-        <v>596</v>
+        <v>307</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B144" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C144" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D144" t="s">
         <v>21</v>
       </c>
       <c r="E144" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="F144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>559</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="D145" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E145" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F145" s="4" t="s">
-        <v>598</v>
+        <v>299</v>
+      </c>
+      <c r="B145" t="s">
+        <v>578</v>
+      </c>
+      <c r="C145" t="s">
+        <v>300</v>
+      </c>
+      <c r="D145" t="s">
+        <v>21</v>
+      </c>
+      <c r="E145" t="s">
+        <v>88</v>
+      </c>
+      <c r="F145" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>600</v>
-      </c>
-      <c r="C146" s="4" t="s">
-        <v>597</v>
-      </c>
-      <c r="D146" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F146" s="4" t="s">
-        <v>599</v>
+        <v>303</v>
+      </c>
+      <c r="B146" t="s">
+        <v>576</v>
+      </c>
+      <c r="C146" t="s">
+        <v>304</v>
+      </c>
+      <c r="D146" t="s">
+        <v>21</v>
+      </c>
+      <c r="E146" t="s">
+        <v>16</v>
+      </c>
+      <c r="F146" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>559</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>314</v>
-      </c>
-      <c r="B149" t="s">
-        <v>360</v>
-      </c>
-      <c r="C149" t="s">
-        <v>315</v>
-      </c>
-      <c r="D149" t="s">
-        <v>21</v>
-      </c>
-      <c r="E149" t="s">
-        <v>16</v>
-      </c>
-      <c r="F149" t="s">
-        <v>333</v>
+        <v>600</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F148" s="4" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>316</v>
-      </c>
-      <c r="B150" t="s">
-        <v>590</v>
-      </c>
-      <c r="C150" t="s">
-        <v>317</v>
-      </c>
-      <c r="D150" t="s">
-        <v>21</v>
-      </c>
-      <c r="E150" t="s">
-        <v>16</v>
-      </c>
-      <c r="F150" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B151" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="C151" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D151" t="s">
         <v>21</v>
@@ -4652,18 +4666,18 @@
         <v>16</v>
       </c>
       <c r="F151" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B152" t="s">
-        <v>314</v>
+        <v>590</v>
       </c>
       <c r="C152" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D152" t="s">
         <v>21</v>
@@ -4672,18 +4686,18 @@
         <v>16</v>
       </c>
       <c r="F152" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B153" t="s">
-        <v>583</v>
+        <v>346</v>
       </c>
       <c r="C153" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D153" t="s">
         <v>21</v>
@@ -4692,18 +4706,18 @@
         <v>16</v>
       </c>
       <c r="F153" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B154" t="s">
-        <v>584</v>
+        <v>314</v>
       </c>
       <c r="C154" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D154" t="s">
         <v>21</v>
@@ -4712,18 +4726,18 @@
         <v>16</v>
       </c>
       <c r="F154" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B155" t="s">
-        <v>366</v>
+        <v>583</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="D155" t="s">
         <v>21</v>
@@ -4732,18 +4746,18 @@
         <v>16</v>
       </c>
       <c r="F155" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B156" t="s">
-        <v>326</v>
+        <v>584</v>
       </c>
       <c r="C156" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D156" t="s">
         <v>21</v>
@@ -4752,18 +4766,18 @@
         <v>16</v>
       </c>
       <c r="F156" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B157" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="C157" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="D157" t="s">
         <v>21</v>
@@ -4772,18 +4786,18 @@
         <v>16</v>
       </c>
       <c r="F157" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B158" t="s">
-        <v>585</v>
+        <v>326</v>
       </c>
       <c r="C158" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D158" t="s">
         <v>21</v>
@@ -4792,63 +4806,63 @@
         <v>16</v>
       </c>
       <c r="F158" t="s">
-        <v>341</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>329</v>
+      </c>
+      <c r="B159" t="s">
+        <v>358</v>
+      </c>
+      <c r="C159" t="s">
+        <v>330</v>
+      </c>
+      <c r="D159" t="s">
+        <v>21</v>
+      </c>
+      <c r="E159" t="s">
+        <v>16</v>
+      </c>
+      <c r="F159" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>344</v>
-      </c>
-      <c r="B161" t="s">
-        <v>324</v>
-      </c>
-      <c r="C161" t="s">
-        <v>345</v>
-      </c>
-      <c r="D161" t="s">
-        <v>21</v>
-      </c>
-      <c r="E161" t="s">
-        <v>16</v>
-      </c>
-      <c r="F161" t="s">
-        <v>378</v>
+        <v>331</v>
+      </c>
+      <c r="B160" t="s">
+        <v>585</v>
+      </c>
+      <c r="C160" t="s">
+        <v>332</v>
+      </c>
+      <c r="D160" t="s">
+        <v>21</v>
+      </c>
+      <c r="E160" t="s">
+        <v>16</v>
+      </c>
+      <c r="F160" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>346</v>
-      </c>
-      <c r="B162" t="s">
-        <v>444</v>
-      </c>
-      <c r="C162" t="s">
-        <v>347</v>
-      </c>
-      <c r="D162" t="s">
-        <v>21</v>
-      </c>
-      <c r="E162" t="s">
-        <v>16</v>
-      </c>
-      <c r="F162" t="s">
-        <v>379</v>
+        <v>343</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B163" t="s">
-        <v>436</v>
+        <v>324</v>
       </c>
       <c r="C163" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D163" t="s">
         <v>21</v>
@@ -4857,18 +4871,18 @@
         <v>16</v>
       </c>
       <c r="F163" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B164" t="s">
-        <v>527</v>
+        <v>444</v>
       </c>
       <c r="C164" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D164" t="s">
         <v>21</v>
@@ -4882,13 +4896,13 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B165" t="s">
-        <v>526</v>
+        <v>436</v>
       </c>
       <c r="C165" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D165" t="s">
         <v>21</v>
@@ -4902,13 +4916,13 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B166" t="s">
-        <v>442</v>
+        <v>527</v>
       </c>
       <c r="C166" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D166" t="s">
         <v>21</v>
@@ -4922,13 +4936,13 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B167" t="s">
-        <v>438</v>
+        <v>526</v>
       </c>
       <c r="C167" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D167" t="s">
         <v>21</v>
@@ -4942,13 +4956,13 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B168" t="s">
-        <v>523</v>
+        <v>442</v>
       </c>
       <c r="C168" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D168" t="s">
         <v>21</v>
@@ -4962,13 +4976,13 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B169" t="s">
-        <v>530</v>
+        <v>438</v>
       </c>
       <c r="C169" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D169" t="s">
         <v>21</v>
@@ -4982,13 +4996,13 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B170" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C170" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D170" t="s">
         <v>21</v>
@@ -5002,13 +5016,13 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B171" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C171" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D171" t="s">
         <v>21</v>
@@ -5022,13 +5036,13 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B172" t="s">
-        <v>533</v>
+        <v>522</v>
       </c>
       <c r="C172" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D172" t="s">
         <v>21</v>
@@ -5042,13 +5056,13 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B173" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="C173" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D173" t="s">
         <v>21</v>
@@ -5062,13 +5076,13 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B174" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="C174" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D174" t="s">
         <v>21</v>
@@ -5082,13 +5096,13 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B175" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C175" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D175" t="s">
         <v>21</v>
@@ -5102,13 +5116,13 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B176" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C176" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D176" t="s">
         <v>21</v>
@@ -5122,13 +5136,13 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B177" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="C177" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D177" t="s">
         <v>21</v>
@@ -5140,60 +5154,60 @@
         <v>379</v>
       </c>
     </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>374</v>
+      </c>
+      <c r="B178" t="s">
+        <v>534</v>
+      </c>
+      <c r="C178" t="s">
+        <v>375</v>
+      </c>
+      <c r="D178" t="s">
+        <v>21</v>
+      </c>
+      <c r="E178" t="s">
+        <v>16</v>
+      </c>
+      <c r="F178" t="s">
+        <v>379</v>
+      </c>
+    </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>380</v>
-      </c>
-      <c r="B180" t="s">
-        <v>548</v>
-      </c>
-      <c r="C180" t="s">
-        <v>381</v>
-      </c>
-      <c r="D180" t="s">
-        <v>21</v>
-      </c>
-      <c r="E180" t="s">
-        <v>16</v>
-      </c>
-      <c r="F180" t="s">
-        <v>453</v>
+        <v>376</v>
+      </c>
+      <c r="B179" t="s">
+        <v>521</v>
+      </c>
+      <c r="C179" t="s">
+        <v>377</v>
+      </c>
+      <c r="D179" t="s">
+        <v>21</v>
+      </c>
+      <c r="E179" t="s">
+        <v>16</v>
+      </c>
+      <c r="F179" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>382</v>
-      </c>
-      <c r="B181" t="s">
-        <v>559</v>
-      </c>
-      <c r="C181" t="s">
-        <v>383</v>
-      </c>
-      <c r="D181" t="s">
-        <v>21</v>
-      </c>
-      <c r="E181" t="s">
-        <v>16</v>
-      </c>
-      <c r="F181" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B182" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C182" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D182" t="s">
         <v>21</v>
@@ -5202,18 +5216,18 @@
         <v>16</v>
       </c>
       <c r="F182" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B183" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C183" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D183" t="s">
         <v>21</v>
@@ -5222,18 +5236,18 @@
         <v>16</v>
       </c>
       <c r="F183" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="B184" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C184" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D184" t="s">
         <v>21</v>
@@ -5242,18 +5256,18 @@
         <v>16</v>
       </c>
       <c r="F184" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B185" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C185" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D185" t="s">
         <v>21</v>
@@ -5262,18 +5276,18 @@
         <v>16</v>
       </c>
       <c r="F185" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B186" t="s">
-        <v>303</v>
+        <v>553</v>
       </c>
       <c r="C186" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D186" t="s">
         <v>21</v>
@@ -5282,18 +5296,18 @@
         <v>16</v>
       </c>
       <c r="F186" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B187" t="s">
-        <v>394</v>
+        <v>557</v>
       </c>
       <c r="C187" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D187" t="s">
         <v>21</v>
@@ -5302,18 +5316,18 @@
         <v>16</v>
       </c>
       <c r="F187" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B188" t="s">
-        <v>556</v>
+        <v>303</v>
       </c>
       <c r="C188" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D188" t="s">
         <v>21</v>
@@ -5322,18 +5336,18 @@
         <v>16</v>
       </c>
       <c r="F188" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B189" t="s">
-        <v>555</v>
+        <v>394</v>
       </c>
       <c r="C189" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D189" t="s">
         <v>21</v>
@@ -5342,18 +5356,18 @@
         <v>16</v>
       </c>
       <c r="F189" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B190" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C190" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D190" t="s">
         <v>21</v>
@@ -5362,18 +5376,18 @@
         <v>16</v>
       </c>
       <c r="F190" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B191" t="s">
-        <v>386</v>
+        <v>555</v>
       </c>
       <c r="C191" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D191" t="s">
         <v>21</v>
@@ -5382,18 +5396,18 @@
         <v>16</v>
       </c>
       <c r="F191" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B192" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="C192" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="D192" t="s">
         <v>21</v>
@@ -5402,18 +5416,18 @@
         <v>16</v>
       </c>
       <c r="F192" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B193" t="s">
-        <v>552</v>
+        <v>386</v>
       </c>
       <c r="C193" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D193" t="s">
         <v>21</v>
@@ -5422,18 +5436,18 @@
         <v>16</v>
       </c>
       <c r="F193" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B194" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="C194" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="D194" t="s">
         <v>21</v>
@@ -5442,18 +5456,18 @@
         <v>16</v>
       </c>
       <c r="F194" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B195" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="C195" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D195" t="s">
         <v>21</v>
@@ -5462,18 +5476,18 @@
         <v>16</v>
       </c>
       <c r="F195" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B196" t="s">
-        <v>390</v>
+        <v>547</v>
       </c>
       <c r="C196" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D196" t="s">
         <v>21</v>
@@ -5482,18 +5496,18 @@
         <v>16</v>
       </c>
       <c r="F196" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B197" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C197" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D197" t="s">
         <v>21</v>
@@ -5502,18 +5516,18 @@
         <v>16</v>
       </c>
       <c r="F197" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B198" t="s">
-        <v>546</v>
+        <v>390</v>
       </c>
       <c r="C198" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D198" t="s">
         <v>21</v>
@@ -5522,18 +5536,18 @@
         <v>16</v>
       </c>
       <c r="F198" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B199" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="C199" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D199" t="s">
         <v>21</v>
@@ -5542,18 +5556,18 @@
         <v>16</v>
       </c>
       <c r="F199" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B200" t="s">
-        <v>404</v>
+        <v>546</v>
       </c>
       <c r="C200" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D200" t="s">
         <v>21</v>
@@ -5562,18 +5576,18 @@
         <v>16</v>
       </c>
       <c r="F200" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B201" t="s">
-        <v>27</v>
+        <v>544</v>
       </c>
       <c r="C201" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D201" t="s">
         <v>21</v>
@@ -5582,18 +5596,18 @@
         <v>16</v>
       </c>
       <c r="F201" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B202" t="s">
-        <v>29</v>
+        <v>404</v>
       </c>
       <c r="C202" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D202" t="s">
         <v>21</v>
@@ -5602,18 +5616,18 @@
         <v>16</v>
       </c>
       <c r="F202" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B203" t="s">
-        <v>380</v>
+        <v>27</v>
       </c>
       <c r="C203" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D203" t="s">
         <v>21</v>
@@ -5622,63 +5636,63 @@
         <v>16</v>
       </c>
       <c r="F203" t="s">
-        <v>465</v>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>424</v>
+      </c>
+      <c r="B204" t="s">
+        <v>29</v>
+      </c>
+      <c r="C204" t="s">
+        <v>425</v>
+      </c>
+      <c r="D204" t="s">
+        <v>21</v>
+      </c>
+      <c r="E204" t="s">
+        <v>16</v>
+      </c>
+      <c r="F204" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>428</v>
-      </c>
-      <c r="B206" t="s">
-        <v>528</v>
-      </c>
-      <c r="C206" t="s">
-        <v>429</v>
-      </c>
-      <c r="D206" t="s">
-        <v>21</v>
-      </c>
-      <c r="E206" t="s">
-        <v>16</v>
-      </c>
-      <c r="F206" t="s">
-        <v>473</v>
+        <v>426</v>
+      </c>
+      <c r="B205" t="s">
+        <v>380</v>
+      </c>
+      <c r="C205" t="s">
+        <v>427</v>
+      </c>
+      <c r="D205" t="s">
+        <v>21</v>
+      </c>
+      <c r="E205" t="s">
+        <v>16</v>
+      </c>
+      <c r="F205" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>430</v>
-      </c>
-      <c r="B207" t="s">
-        <v>542</v>
-      </c>
-      <c r="C207" t="s">
-        <v>431</v>
-      </c>
-      <c r="D207" t="s">
-        <v>21</v>
-      </c>
-      <c r="E207" t="s">
-        <v>16</v>
-      </c>
-      <c r="F207" t="s">
-        <v>474</v>
+        <v>449</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B208" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="C208" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D208" t="s">
         <v>21</v>
@@ -5687,18 +5701,18 @@
         <v>16</v>
       </c>
       <c r="F208" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B209" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C209" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D209" t="s">
         <v>21</v>
@@ -5707,18 +5721,18 @@
         <v>16</v>
       </c>
       <c r="F209" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B210" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C210" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D210" t="s">
         <v>21</v>
@@ -5727,18 +5741,18 @@
         <v>16</v>
       </c>
       <c r="F210" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B211" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="C211" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D211" t="s">
         <v>21</v>
@@ -5747,18 +5761,18 @@
         <v>16</v>
       </c>
       <c r="F211" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B212" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C212" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D212" t="s">
         <v>21</v>
@@ -5767,18 +5781,18 @@
         <v>16</v>
       </c>
       <c r="F212" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B213" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C213" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D213" t="s">
         <v>21</v>
@@ -5787,18 +5801,18 @@
         <v>16</v>
       </c>
       <c r="F213" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B214" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C214" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D214" t="s">
         <v>21</v>
@@ -5807,31 +5821,71 @@
         <v>16</v>
       </c>
       <c r="F214" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
+        <v>442</v>
+      </c>
+      <c r="B215" t="s">
+        <v>538</v>
+      </c>
+      <c r="C215" t="s">
+        <v>443</v>
+      </c>
+      <c r="D215" t="s">
+        <v>21</v>
+      </c>
+      <c r="E215" t="s">
+        <v>16</v>
+      </c>
+      <c r="F215" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>444</v>
+      </c>
+      <c r="B216" t="s">
+        <v>539</v>
+      </c>
+      <c r="C216" t="s">
+        <v>445</v>
+      </c>
+      <c r="D216" t="s">
+        <v>21</v>
+      </c>
+      <c r="E216" t="s">
+        <v>16</v>
+      </c>
+      <c r="F216" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>446</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B217" t="s">
         <v>536</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C217" t="s">
         <v>447</v>
       </c>
-      <c r="D215" t="s">
-        <v>21</v>
-      </c>
-      <c r="E215" t="s">
-        <v>16</v>
-      </c>
-      <c r="F215" t="s">
+      <c r="D217" t="s">
+        <v>21</v>
+      </c>
+      <c r="E217" t="s">
+        <v>16</v>
+      </c>
+      <c r="F217" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C218" t="s">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C220" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>